<commit_message>
New files for iteration 1
</commit_message>
<xml_diff>
--- a/doc/CS673_SPPP_RiskManagement.xlsx
+++ b/doc/CS673_SPPP_RiskManagement.xlsx
@@ -17,10 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
-  <si>
-    <t>This sheet provides some common risks in student projects. You should check if it applies to your group project. 
-You should also feel free to add other risks. Exemplary analysis is also added.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="123">
+  <si>
+    <t>}</t>
   </si>
   <si>
     <t>Risk Category</t>
@@ -385,6 +384,10 @@
   </si>
   <si>
     <t>Time allocated in project plan</t>
+  </si>
+  <si>
+    <t>This sheet provides some common risks in student projects. You should check if it applies to your group project. 
+You should also feel free to add other risks. Exemplary analysis is also added.</t>
   </si>
   <si>
     <t>The team member who is adding the new feature should be the one who determines what is correct for the new functionality that was added.</t>
@@ -458,12 +461,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -516,6 +519,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -748,7 +754,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.63"/>
     <col customWidth="1" min="2" max="2" width="22.25"/>
-    <col customWidth="1" min="3" max="3" width="25.75"/>
+    <col customWidth="1" min="3" max="3" width="37.38"/>
     <col customWidth="1" min="4" max="4" width="8.88"/>
     <col customWidth="1" min="5" max="5" width="10.13"/>
     <col customWidth="1" min="6" max="7" width="10.88"/>
@@ -3585,8 +3591,8 @@
   </cols>
   <sheetData>
     <row r="1" ht="37.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3644,35 +3650,35 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="22">
         <v>2.0</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="22">
         <v>4.0</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="22">
         <v>4.0</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="22">
         <f>(6-D3)*(6-E3)*F3</f>
         <v>32</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="23">
         <v>44713.0</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="21" t="s">
         <v>19</v>
       </c>
       <c r="M3" s="7"/>
@@ -4765,7 +4771,7 @@
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
@@ -4796,7 +4802,7 @@
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>

</xml_diff>